<commit_message>
Formatting. Happy with it.
</commit_message>
<xml_diff>
--- a/tables/23-sediment_biogeochemistry/BookdownParams.xlsx
+++ b/tables/23-sediment_biogeochemistry/BookdownParams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00074264\AED Dropbox\AED_Coorong_db\5_reporting\CDM Manual\DanDrafts\aed-science\tables\23-sediment_biogeochemistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794BCA34-D72F-4A2B-A057-5FF2DA3502F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AE885C-34F8-4727-A4FD-6312FDB552D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31320" yWindow="-2970" windowWidth="26400" windowHeight="16440" tabRatio="744" activeTab="9" xr2:uid="{D0F3A7CD-BCCC-46D9-BB4D-8BBA552EBE79}"/>
+    <workbookView xWindow="31320" yWindow="-2970" windowWidth="26400" windowHeight="16440" tabRatio="744" activeTab="12" xr2:uid="{D0F3A7CD-BCCC-46D9-BB4D-8BBA552EBE79}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -66234,11 +66234,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9BB1EA-8267-4BD4-AE3F-8F599A64EE13}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C47" sqref="C47"/>
+      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -67144,7 +67144,7 @@
   <dimension ref="A1:C281"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -71095,8 +71095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C17420C3-0336-481E-83D4-F3D7AC33D995}">
   <dimension ref="A1:N410"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A270" workbookViewId="0">
+      <selection activeCell="A289" sqref="A289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
First set of Matt edits
</commit_message>
<xml_diff>
--- a/tables/23-sediment_biogeochemistry/BookdownParams.xlsx
+++ b/tables/23-sediment_biogeochemistry/BookdownParams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00074264\AED Dropbox\AED_Coorong_db\5_reporting\CDM Manual\DanDrafts\aed-science\tables\23-sediment_biogeochemistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AE885C-34F8-4727-A4FD-6312FDB552D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75282C33-02EA-4FB7-ABA6-9F204CB488A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31320" yWindow="-2970" windowWidth="26400" windowHeight="16440" tabRatio="744" activeTab="12" xr2:uid="{D0F3A7CD-BCCC-46D9-BB4D-8BBA552EBE79}"/>
+    <workbookView xWindow="31485" yWindow="-2970" windowWidth="26235" windowHeight="16440" tabRatio="744" activeTab="12" xr2:uid="{D0F3A7CD-BCCC-46D9-BB4D-8BBA552EBE79}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Started the Setup examples
</commit_message>
<xml_diff>
--- a/tables/23-sediment_biogeochemistry/BookdownParams.xlsx
+++ b/tables/23-sediment_biogeochemistry/BookdownParams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00074264\AED Dropbox\AED_Coorong_db\5_reporting\CDM Manual\DanDrafts\aed-science\tables\23-sediment_biogeochemistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8938AC6-5D9E-40FB-AB85-EFC074786B05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF53319E-C6AF-4DDD-977F-56025698A109}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31515" yWindow="-2970" windowWidth="26205" windowHeight="16440" tabRatio="744" activeTab="12" xr2:uid="{D0F3A7CD-BCCC-46D9-BB4D-8BBA552EBE79}"/>
+    <workbookView xWindow="60135" yWindow="-1335" windowWidth="26385" windowHeight="16440" tabRatio="744" activeTab="9" xr2:uid="{D0F3A7CD-BCCC-46D9-BB4D-8BBA552EBE79}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="570">
   <si>
     <t>popu</t>
   </si>
@@ -1738,6 +1738,27 @@
   <si>
     <t>(1,2,3)</t>
   </si>
+  <si>
+    <t>Timing parameters</t>
+  </si>
+  <si>
+    <t>Zone setup parameters</t>
+  </si>
+  <si>
+    <t>External parameter file paths</t>
+  </si>
+  <si>
+    <t>Boundary condition parameters and files</t>
+  </si>
+  <si>
+    <t>Initial condition setup</t>
+  </si>
+  <si>
+    <t>Output settings</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
 </sst>
 </file>
 
@@ -66232,13 +66253,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9BB1EA-8267-4BD4-AE3F-8F599A64EE13}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -66246,12 +66267,12 @@
     <col min="1" max="1" width="37" customWidth="1"/>
     <col min="2" max="2" width="73.140625" customWidth="1"/>
     <col min="3" max="3" width="59.140625" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.7109375" customWidth="1"/>
     <col min="6" max="6" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>392</v>
       </c>
@@ -66261,283 +66282,373 @@
       <c r="C1" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>472</v>
-      </c>
-      <c r="B2">
+        <v>400</v>
+      </c>
+      <c r="B2" t="str">
         <f>VLOOKUP($A2,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Duration of spinup before flux (d)</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B3" t="str">
         <f>VLOOKUP($A3,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>Duration of spinup before flux (d)</v>
+        <v>Hydrodynamic model time step (s)</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>900</v>
+      </c>
+      <c r="D3" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B4" t="str">
         <f>VLOOKUP($A4,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>Hydrodynamic model time step (s)</v>
+        <v>Sediment model substep (h)</v>
       </c>
       <c r="C4">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>399</v>
+        <v>435</v>
       </c>
       <c r="B5" t="str">
         <f>VLOOKUP($A5,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>Sediment model substep (h)</v>
+        <v>Number of zones to simulate. Zones are listed in `active_zones` (integer)</v>
       </c>
       <c r="C5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>473</v>
+        <v>436</v>
       </c>
       <c r="B6" t="str">
         <f>VLOOKUP($A6,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Sequence of zones to be simulated (integer)</v>
+      </c>
+      <c r="C6" t="s">
+        <v>437</v>
+      </c>
+      <c r="D6" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B7" t="str">
         <f>VLOOKUP($A7,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>Number of zones to simulate. Zones are listed in `active_zones` (integer)</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Type of zone, as listed by header in aed_sdg_vars.csv (integer)</v>
+      </c>
+      <c r="C7" t="s">
+        <v>439</v>
+      </c>
+      <c r="D7" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="B8" t="str">
         <f>VLOOKUP($A8,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>Sequence of zones to be simulated (integer)</v>
+        <v>External candi parameter file path (text)</v>
       </c>
       <c r="C8" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>441</v>
+      </c>
+      <c r="D8" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>438</v>
-      </c>
-      <c r="B9" t="str">
+        <v>442</v>
+      </c>
+      <c r="B9" t="e">
         <f>VLOOKUP($A9,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>Type of zone, as listed by header in aed_sdg_vars.csv (integer)</v>
+        <v>#N/A</v>
       </c>
       <c r="C9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>443</v>
+      </c>
+      <c r="D9" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>475</v>
+        <v>444</v>
       </c>
       <c r="B10" t="str">
         <f>VLOOKUP($A10,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>External equilibrium chemistry solver parameter file path (text)</v>
+      </c>
+      <c r="C10" t="s">
+        <v>445</v>
+      </c>
+      <c r="D10" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>440</v>
+        <v>418</v>
       </c>
       <c r="B11" t="str">
         <f>VLOOKUP($A11,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>External candi parameter file path (text)</v>
-      </c>
-      <c r="C11" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">Sediment-water interface boundary switch </v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>442</v>
-      </c>
-      <c r="B12" t="e">
+        <v>419</v>
+      </c>
+      <c r="B12" t="str">
         <f>VLOOKUP($A12,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C12" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">Bottom boundary switch </v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B13" t="str">
         <f>VLOOKUP($A13,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>External equilibrium chemistry solver parameter file path (text)</v>
-      </c>
-      <c r="C13" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Sediment-water interface boundary file path (text)</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>476</v>
+      </c>
+      <c r="D13" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>474</v>
+        <v>447</v>
       </c>
       <c r="B14" t="str">
         <f>VLOOKUP($A14,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Deep boundary file path (text)</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>477</v>
+      </c>
+      <c r="D14" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="B15" t="str">
         <f>VLOOKUP($A15,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v xml:space="preserve">Sediment-water interface boundary switch </v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">Variables taken from external boundary file for sediment-water interface </v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="D15" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>419</v>
-      </c>
-      <c r="B16" t="str">
+        <v>421</v>
+      </c>
+      <c r="B16">
         <f>VLOOKUP($A16,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v xml:space="preserve">Bottom boundary switch </v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>448</v>
+      </c>
+      <c r="D16" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="B17" t="str">
         <f>VLOOKUP($A17,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>Sediment-water interface boundary file path (text)</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C17" t="s">
+        <v>450</v>
+      </c>
+      <c r="D17" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="B18" t="str">
         <f>VLOOKUP($A18,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>Deep boundary file path (text)</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Switch for labile organic matter initial profile (constant, linear or exponential) (character switch)</v>
+      </c>
+      <c r="C18" t="s">
+        <v>452</v>
+      </c>
+      <c r="D18" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>420</v>
+        <v>453</v>
       </c>
       <c r="B19" t="str">
         <f>VLOOKUP($A19,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v xml:space="preserve">Variables taken from external boundary file for sediment-water interface </v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Fraction of initial condition at the top of the labile initial profile using linear option (0 to 1)</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>421</v>
-      </c>
-      <c r="B20">
+        <v>454</v>
+      </c>
+      <c r="B20" t="str">
         <f>VLOOKUP($A20,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Fraction of initial condition at the depth InitMinDepthL using linear option (0 to 1)</v>
+      </c>
+      <c r="C20">
+        <v>0.9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>479</v>
+        <v>455</v>
       </c>
       <c r="B21" t="str">
         <f>VLOOKUP($A21,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Decay coefficient for labile organic matter initial profile using exponential option (-)</v>
+      </c>
+      <c r="C21">
+        <v>0.6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>449</v>
+        <v>456</v>
       </c>
       <c r="B22" t="str">
         <f>VLOOKUP($A22,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C22" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Depth at which the OM_minL percentage applies using the linear option (cm)</v>
+      </c>
+      <c r="C22">
+        <v>99</v>
+      </c>
+      <c r="D22" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>451</v>
+        <v>457</v>
       </c>
       <c r="B23" t="str">
         <f>VLOOKUP($A23,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>Switch for labile organic matter initial profile (constant, linear or exponential) (character switch)</v>
+        <v>Switch for refractory organic matter initial profile (constant, linear or exponential) (character switch)</v>
       </c>
       <c r="C23" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>453</v>
+        <v>458</v>
       </c>
       <c r="B24" t="str">
         <f>VLOOKUP($A24,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>Fraction of initial condition at the top of the labile initial profile using linear option (0 to 1)</v>
+        <v>Fraction of initial condition at the top of the refractory initial profile using linear option (0 to 1)</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
       <c r="B25" t="str">
         <f>VLOOKUP($A25,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>Fraction of initial condition at the depth InitMinDepthL using linear option (0 to 1)</v>
+        <v>Fraction of initial condition at the depth InitMinDepthR using linear option (0 to 1)</v>
       </c>
       <c r="C25">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>455</v>
+        <v>460</v>
       </c>
       <c r="B26" t="str">
         <f>VLOOKUP($A26,lookup!$A$1:$D$499,4,FALSE)</f>
@@ -66546,170 +66657,128 @@
       <c r="C26">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>456</v>
+        <v>461</v>
       </c>
       <c r="B27" t="str">
         <f>VLOOKUP($A27,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>Depth at which the OM_minL percentage applies using the linear option (cm)</v>
+        <v>Depth at which the OM_minR percentage applies using the linear option (cm)</v>
       </c>
       <c r="C27">
         <v>99</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>457</v>
+        <v>462</v>
       </c>
       <c r="B28" t="str">
         <f>VLOOKUP($A28,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>Switch for refractory organic matter initial profile (constant, linear or exponential) (character switch)</v>
-      </c>
-      <c r="C28" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Concentration of very refractory particulate organic matter (% solids)</v>
+      </c>
+      <c r="C28">
+        <v>0.3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
       <c r="B29" t="str">
         <f>VLOOKUP($A29,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>Fraction of initial condition at the top of the refractory initial profile using linear option (0 to 1)</v>
+        <v>Switch for which types of diags to write to files (integer)</v>
       </c>
       <c r="C29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="D29" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>459</v>
+        <v>464</v>
       </c>
       <c r="B30" t="str">
         <f>VLOOKUP($A30,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>Fraction of initial condition at the depth InitMinDepthR using linear option (0 to 1)</v>
-      </c>
-      <c r="C30">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Switch to write .sed files (logical)</v>
+      </c>
+      <c r="C30" t="s">
+        <v>465</v>
+      </c>
+      <c r="D30" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>460</v>
+        <v>466</v>
       </c>
       <c r="B31" t="str">
         <f>VLOOKUP($A31,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>Decay coefficient for labile organic matter initial profile using exponential option (-)</v>
-      </c>
-      <c r="C31">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>List of other variables to be written to output files e.g. rates, factors etc. (text)</v>
+      </c>
+      <c r="C31" t="s">
+        <v>467</v>
+      </c>
+      <c r="D31" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="B32" t="str">
         <f>VLOOKUP($A32,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>Depth at which the OM_minR percentage applies using the linear option (cm)</v>
-      </c>
-      <c r="C32">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>List of variables to be written to diag files at `output_diag_depths` (text)</v>
+      </c>
+      <c r="C32" t="s">
+        <v>469</v>
+      </c>
+      <c r="D32" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>462</v>
+        <v>470</v>
       </c>
       <c r="B33" t="str">
         <f>VLOOKUP($A33,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>Concentration of very refractory particulate organic matter (% solids)</v>
+        <v>Number of depths to write diag outputs for. Depths are listed in `output_diag_depths` (integer)</v>
       </c>
       <c r="C33">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
       <c r="B34" t="str">
         <f>VLOOKUP($A34,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>463</v>
-      </c>
-      <c r="B35" t="str">
-        <f>VLOOKUP($A35,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>Switch for which types of diags to write to files (integer)</v>
-      </c>
-      <c r="C35">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>464</v>
-      </c>
-      <c r="B36" t="str">
-        <f>VLOOKUP($A36,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>Switch to write .sed files (logical)</v>
-      </c>
-      <c r="C36" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>466</v>
-      </c>
-      <c r="B37" t="str">
-        <f>VLOOKUP($A37,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>List of other variables to be written to output files e.g. rates, factors etc. (text)</v>
-      </c>
-      <c r="C37" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>468</v>
-      </c>
-      <c r="B38" t="str">
-        <f>VLOOKUP($A38,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>List of variables to be written to diag files at `output_diag_depths` (text)</v>
-      </c>
-      <c r="C38" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>470</v>
-      </c>
-      <c r="B39" t="str">
-        <f>VLOOKUP($A39,lookup!$A$1:$D$499,4,FALSE)</f>
-        <v>Number of depths to write diag outputs for. Depths are listed in `output_diag_depths` (integer)</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>471</v>
-      </c>
-      <c r="B40" t="str">
-        <f>VLOOKUP($A40,lookup!$A$1:$D$499,4,FALSE)</f>
         <v>Depths to write diag files (cm)</v>
       </c>
-      <c r="C40">
-        <v>1</v>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>568</v>
       </c>
     </row>
   </sheetData>
@@ -71095,7 +71164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C17420C3-0336-481E-83D4-F3D7AC33D995}">
   <dimension ref="A1:N410"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
+    <sheetView topLeftCell="A307" workbookViewId="0">
       <selection activeCell="B376" sqref="B376"/>
     </sheetView>
   </sheetViews>

</xml_diff>